<commit_message>
sesion de hoy de scraping
</commit_message>
<xml_diff>
--- a/02_web_scraping/scraping_cannes/cannes_seccion_oficial_wiki_con_paises_y_enlaces.xlsx
+++ b/02_web_scraping/scraping_cannes/cannes_seccion_oficial_wiki_con_paises_y_enlaces.xlsx
@@ -15439,12 +15439,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_-* #,##0\ &quot;€&quot;_-;\-* #,##0\ &quot;€&quot;_-;_-* &quot;-&quot;\ &quot;€&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="176" formatCode="_-* #,##0\ &quot;€&quot;_-;\-* #,##0\ &quot;€&quot;_-;_-* &quot;-&quot;\ &quot;€&quot;_-;_-@_-"/>
+    <numFmt numFmtId="177" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* \-??\ &quot;€&quot;_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="177" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* \-??\ &quot;€&quot;_-;_-@_-"/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -15476,34 +15476,10 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -15529,29 +15505,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color theme="3"/>
@@ -15567,9 +15520,47 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -15583,8 +15574,17 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -15598,14 +15598,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -15620,13 +15613,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -15638,19 +15643,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -15662,25 +15655,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -15698,19 +15679,79 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -15728,37 +15769,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -15776,31 +15793,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -15825,32 +15818,6 @@
       </top>
       <bottom style="thin">
         <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -15903,6 +15870,32 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -15929,145 +15922,145 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="14" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="18" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="14" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -16079,7 +16072,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="48"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="48" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -16429,10 +16422,13 @@
   <dimension ref="A1:G1661"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="6"/>
+  <cols>
+    <col min="6" max="6" width="18.5" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">

</xml_diff>